<commit_message>
alterando feature selecionar os serviçoes web
</commit_message>
<xml_diff>
--- a/DATABASE/database.xlsx
+++ b/DATABASE/database.xlsx
@@ -655,7 +655,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -668,6 +668,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1055,473 +1058,466 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="10.2857142857143" defaultRowHeight="12.75"/>
-  <cols>
-    <col width="76" customWidth="1" style="1" min="1" max="1"/>
-    <col width="17.5714285714286" customWidth="1" style="1" min="2" max="2"/>
-    <col width="24.4285714285714" customWidth="1" style="1" min="3" max="3"/>
-    <col width="9.28571428571429" customWidth="1" style="1" min="4" max="4"/>
-    <col width="44.4285714285714" customWidth="1" style="1" min="5" max="5"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>TITULO</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>EDITAL</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>COORDENADOR</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>SIAPE</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>LOTAÇÃO</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Cidades Inteligentes: Metamodelo de Tratamento da Sustentável da Sucata Eletrônica.</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>FACEPE N. 28/2022</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Sidney Marlon Lopes de Lima</t>
         </is>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" t="n">
         <v>1891425</v>
       </c>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Departamento de Eletrônica e Sistemas, CTG/UFPE</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>hrushrishur</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>djakldjad</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>djlakldad</t>
         </is>
       </c>
-      <c r="D3" s="4" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>khdkahdjas</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>xkljzdkzld</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>dklsnldksd</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>jkldajkda</t>
         </is>
       </c>
-      <c r="C4" s="4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>kldjksljdksad</t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>jldsjkdjlsd</t>
         </is>
       </c>
-      <c r="E4" s="3" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>jkdljsldksad</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>jdklsjdks</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>ndjklhkjl</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>jdzhkdhjz</t>
         </is>
       </c>
-      <c r="D5" s="4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>hjdkzhjdkzd</t>
         </is>
       </c>
-      <c r="E5" s="3" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>dhzldkjzdz</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Produção e Consumo Responsáveis da Arte Figurativa no Alto do Moura - ProCRAFAM</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>FACEPE 28/2022</t>
         </is>
       </c>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Profa. Julia Santos Bezerra de Menezes</t>
         </is>
       </c>
-      <c r="D6" s="4" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>56903949</t>
         </is>
       </c>
-      <c r="E6" s="3" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Departamento de Antropologia</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>hrushrishur</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>FACEPE 28/2022</t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>kelwkejlsed</t>
         </is>
       </c>
-      <c r="D7" s="4" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>456566666</t>
         </is>
       </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Departamento de Antropologia</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Projeto Math Ansud</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>FACEPE 28/2022</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Pablo de Tarso Ferreira Junior Campos de Barros</t>
         </is>
       </c>
-      <c r="D8" s="4" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>02496068026</t>
         </is>
       </c>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Departamento de Antropologia</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>ddddd</t>
         </is>
       </c>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>FACEPE 28/2022d</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>dddsads</t>
         </is>
       </c>
-      <c r="D9" s="4" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>dsdsds</t>
         </is>
       </c>
-      <c r="E9" s="3" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>dsdsds</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>ssfds</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>FACEPE 28/2022</t>
         </is>
       </c>
-      <c r="C10" s="4" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Pablo de Tarso Ferreira Junior Campos de Barros</t>
         </is>
       </c>
-      <c r="D10" s="4" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>02496068026</t>
         </is>
       </c>
-      <c r="E10" s="3" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>Departamento de Antropologia</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>ssfds</t>
         </is>
       </c>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>FACEPE 28/2022</t>
         </is>
       </c>
-      <c r="C11" s="4" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Pablo de Tarso Ferreira Junior Campos de Barros</t>
         </is>
       </c>
-      <c r="D11" s="4" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>02496068026</t>
         </is>
       </c>
-      <c r="E11" s="3" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>Departamento de Antropologia</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>dklsnldksd</t>
         </is>
       </c>
-      <c r="B12" s="3" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>FACEPE 28/2022</t>
         </is>
       </c>
-      <c r="C12" s="4" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>Profa. Julia Santos Bezerra de Menezes</t>
         </is>
       </c>
-      <c r="D12" s="4" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>456566666</t>
         </is>
       </c>
-      <c r="E12" s="3" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>Departamento de Antropologia</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Estratégias de prevenção à violência e de promoção da saúde mental no contexto escolar: revisão sistemática</t>
         </is>
       </c>
-      <c r="B13" s="3" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>FACEPE 28/2022</t>
         </is>
       </c>
-      <c r="C13" s="4" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>Jaqueline Galdino Albuquerque Perrelli</t>
         </is>
       </c>
-      <c r="D13" s="4" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>1657188</t>
         </is>
       </c>
-      <c r="E13" s="3" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>Departamento de Enfermagem, Centro de Ciências da Saúde, Campus Recife</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Orçamento sensível e partilha do cuidado na capital das mulheres: o papel do Município na promoção de um mercado de trabalho mais justo e igualitário para as Recifenses</t>
         </is>
       </c>
-      <c r="B14" s="3" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>FACEPE 28/2022</t>
         </is>
       </c>
-      <c r="C14" s="4" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>Prof.ª Dr.ª Juliana Teixeira Esteves</t>
         </is>
       </c>
-      <c r="D14" s="4" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>4347617</t>
         </is>
       </c>
-      <c r="E14" s="3" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>Coordenação da graduação em Direito - FDR - Centro de Ciências Jurídicas - CCJ</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="inlineStr">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Tony Meireles dos Santos</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>FACEPE 28/2022</t>
         </is>
       </c>
-      <c r="C15" s="4" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Capacitação de Recursos Humanos para Prescrição de Exercícios para Sobreviventes de  Câncer</t>
         </is>
       </c>
-      <c r="D15" s="4" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t xml:space="preserve">1999436 </t>
         </is>
       </c>
-      <c r="E15" s="3" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t xml:space="preserve">Departamento de Educação Física, Centro de Ciências da Saúde, Campus Recife. </t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Capacitação de Recursos Humanos para Prescrição de Exercícios para Sobreviventes de  Câncer</t>
         </is>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B16" t="inlineStr">
         <is>
           <t>FACEPE 28/2022</t>
         </is>
       </c>
-      <c r="C16" s="4" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>Tony Meireles dos Santos</t>
         </is>
       </c>
-      <c r="D16" s="4" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>1999436</t>
         </is>
       </c>
-      <c r="E16" s="3" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>Departamento de Educação Física, Centro de Ciências da Saúde, Campus Recife</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="inlineStr">
+      <c r="A17" t="inlineStr">
         <is>
           <t>Consolidação  de uma base de dados ecológicos para estabelecimento de estratégias sustentáveis de  uso e cobertura do solo em áreas de uso forrageiro no Bioma Caatinga</t>
         </is>
       </c>
-      <c r="B17" s="3" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>FACEPE Nº  28/2022</t>
         </is>
       </c>
-      <c r="C17" s="4" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>Ana Dolores Santiago de  Freitas</t>
         </is>
       </c>
-      <c r="D17" s="4" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>382959</t>
         </is>
       </c>
-      <c r="E17" s="3" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>Universidade Federal Rural de Pernambuco (UFRPE), e assumimos o compromisso de apoiar  o desenvolvimento do referido projeto a ser realizado no período de 01/12/ 2022 a 01/05/2024</t>
         </is>
@@ -1551,6 +1547,33 @@
       <c r="E18" t="inlineStr">
         <is>
           <t>DEPARTAMENTO DE FÍSICA, Centro de Ciências Exatas e da Natureza - CCEN, CAMPUS RECIFE - UFPE</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ejoajiajoejiaoejiaojeoia</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>FACEPE 59/2022</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Thiago Borges Miranda</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>506070</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Dep Fisica</t>
         </is>
       </c>
     </row>

</xml_diff>